<commit_message>
refactoring before new report
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -523,12 +523,12 @@
       </c>
       <c r="G3" s="3" t="inlineStr">
         <is>
-          <t>кол-во выполненное</t>
+          <t>кол-во факт</t>
         </is>
       </c>
       <c r="H3" s="3" t="inlineStr">
         <is>
-          <t>сумма_заказчика</t>
+          <t>сумма факт</t>
         </is>
       </c>
     </row>
@@ -658,12 +658,12 @@
       </c>
       <c r="G9" s="3" t="inlineStr">
         <is>
-          <t>кол-во выполненное</t>
+          <t>кол-во факт</t>
         </is>
       </c>
       <c r="H9" s="3" t="inlineStr">
         <is>
-          <t>сумма_заказчика</t>
+          <t>сумма факт</t>
         </is>
       </c>
     </row>
@@ -750,7 +750,7 @@
       <c r="A15" s="5" t="n"/>
       <c r="B15" s="5" t="inlineStr">
         <is>
-          <t>По объекту</t>
+          <t>ИТОГО по объекту</t>
         </is>
       </c>
       <c r="C15" s="5" t="n"/>

</xml_diff>